<commit_message>
update GotionBattery to add download/upload function
</commit_message>
<xml_diff>
--- a/D8dashboard/GotionBattery/8Dtemplate.xlsx
+++ b/D8dashboard/GotionBattery/8Dtemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t.li\BatteryData\lib\BatteryLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4738F3A0-000F-45E0-A317-4D9DEFE49832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00B4914-123A-485F-8404-2BD13E5C1314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14145" yWindow="5790" windowWidth="28800" windowHeight="15435" activeTab="10" xr2:uid="{5BFB07E2-966C-4A49-BF6A-755BA9666F75}"/>
+    <workbookView xWindow="-21075" yWindow="3870" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{5BFB07E2-966C-4A49-BF6A-755BA9666F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Coversheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Supplier</t>
   </si>
@@ -376,9 +376,6 @@
     <t>D1</t>
   </si>
   <si>
-    <t>Evidence / Notes</t>
-  </si>
-  <si>
     <t>Cause</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
       </rPr>
       <t>Acknowledge / recognize team, celebrate successful completion, ensure documentation/information storage is completed for easy retrieval, review metrics for identification of next opportunity.</t>
     </r>
-  </si>
-  <si>
-    <t>Name / Signature</t>
   </si>
   <si>
     <t>Telephone #</t>
@@ -631,6 +625,9 @@
   </si>
   <si>
     <t>Date_Due</t>
+  </si>
+  <si>
+    <t>Evidence/Notes</t>
   </si>
 </sst>
 </file>
@@ -862,7 +859,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -892,19 +889,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1273,90 +1257,81 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thick">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thick">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1364,207 +1339,195 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1944,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310ADA72-F2C7-4A04-9315-1DEA32E9B512}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,7 +1937,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>33</v>
@@ -1982,7 +1945,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>34</v>
@@ -1990,74 +1953,74 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2100,46 +2063,49 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3341F06A-DAB9-414D-BE90-2037BF5DBF4D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="18" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="E1" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="58">
+        <v>43818</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2150,9 +2116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2431E8-D233-433C-917D-1B156F088116}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2164,224 +2128,227 @@
     <col min="6" max="6" width="15.42578125" style="18" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45">
+        <v>43806</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="45">
+        <v>43807</v>
+      </c>
+      <c r="E2" s="45">
+        <v>43807</v>
+      </c>
+      <c r="F2" s="45">
+        <v>43807</v>
+      </c>
+      <c r="G2" s="45" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47">
+      <c r="H2" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45">
+        <v>43807</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="49">
+        <v>43808</v>
+      </c>
+      <c r="E3" s="49">
+        <v>43808</v>
+      </c>
+      <c r="F3" s="49">
+        <v>43808</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45">
+        <v>43807</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="49">
+        <v>43808</v>
+      </c>
+      <c r="E4" s="49">
+        <v>43808</v>
+      </c>
+      <c r="F4" s="49">
+        <v>43808</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45">
         <v>43806</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B5" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="48">
+        <v>43809</v>
+      </c>
+      <c r="E5" s="48">
+        <v>43809</v>
+      </c>
+      <c r="F5" s="48">
+        <v>43809</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="47">
-        <v>43807</v>
-      </c>
-      <c r="E2" s="47">
-        <v>43807</v>
-      </c>
-      <c r="F2" s="47">
-        <v>43807</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47">
-        <v>43807</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="51">
-        <v>43808</v>
-      </c>
-      <c r="E3" s="51">
-        <v>43808</v>
-      </c>
-      <c r="F3" s="51">
-        <v>43808</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47">
-        <v>43807</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="51">
-        <v>43808</v>
-      </c>
-      <c r="E4" s="51">
-        <v>43808</v>
-      </c>
-      <c r="F4" s="51">
-        <v>43808</v>
-      </c>
-      <c r="G4" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47">
+    </row>
+    <row r="6" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45">
+        <v>43809</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="49">
+        <v>43809</v>
+      </c>
+      <c r="E6" s="49">
+        <v>43809</v>
+      </c>
+      <c r="F6" s="49">
+        <v>43809</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="45">
         <v>43806</v>
       </c>
-      <c r="B5" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="50">
+      <c r="B7" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45">
+        <v>43806</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="49">
         <v>43809</v>
       </c>
-      <c r="E5" s="50">
-        <v>43809</v>
-      </c>
-      <c r="F5" s="50">
-        <v>43809</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47">
-        <v>43809</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="51">
-        <v>43809</v>
-      </c>
-      <c r="E6" s="51">
-        <v>43809</v>
-      </c>
-      <c r="F6" s="51">
-        <v>43809</v>
-      </c>
-      <c r="G6" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47">
-        <v>43806</v>
-      </c>
-      <c r="B7" s="49" t="s">
+      <c r="E8" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47">
-        <v>43806</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="51">
-        <v>43809</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2403,9 +2370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AA10F3-F822-4290-9938-3734B5B16F66}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2415,7 +2380,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="91.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>6</v>
@@ -2434,15 +2399,15 @@
         <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2450,18 +2415,18 @@
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14"/>
     </row>
@@ -2479,7 +2444,7 @@
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="15">
         <v>43806</v>
@@ -2487,13 +2452,13 @@
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="15">
         <v>43809</v>
@@ -2511,7 +2476,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,7 +2510,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>15</v>
@@ -2568,10 +2533,10 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="70.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="45.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2638,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88737380-9B8B-496B-BA78-2BA14F64701E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,13 +2617,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="87.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="308.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2757,10 +2722,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DB260E-C5E1-44C3-9E8F-42B938FBD43B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,32 +2742,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+    <row r="2" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="56" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="61"/>
-    </row>
-    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B3" s="26" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2823,7 +2779,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="105.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>19</v>
@@ -2835,7 +2791,6 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>